<commit_message>
highlight data from this paper with yellow background
</commit_message>
<xml_diff>
--- a/data/sciimmunol.abl7482_data_source.xlsx
+++ b/data/sciimmunol.abl7482_data_source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yd973/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yd973/Documents/research/Macrophage_framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6C35E6-BFF6-BD42-8562-239785D94777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BD4B1D-7995-3C40-9416-904FFD2AE247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1195,12 +1195,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -1256,7 +1262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1311,8 +1317,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1329,28 +1350,58 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1660,7 +1711,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD19"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1678,24 +1729,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="56.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="30.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1719,10 +1770,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
@@ -1745,65 +1796,65 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="39.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:10" s="36" customFormat="1" ht="39.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:10" s="36" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="35" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="11" t="s">
         <v>28</v>
       </c>
@@ -1827,10 +1878,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
         <v>35</v>
       </c>
@@ -1854,10 +1905,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="14" t="s">
         <v>28</v>
       </c>
@@ -1881,10 +1932,10 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="39.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="27"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
         <v>22</v>
       </c>
@@ -1908,10 +1959,10 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="27"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
         <v>54</v>
       </c>
@@ -1935,10 +1986,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="27"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="14" t="s">
         <v>22</v>
       </c>
@@ -1962,10 +2013,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="27"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="14" t="s">
         <v>22</v>
       </c>
@@ -1989,10 +2040,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="39.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="14" t="s">
         <v>22</v>
       </c>
@@ -2016,10 +2067,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="27"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="11" t="s">
         <v>80</v>
       </c>
@@ -2042,50 +2093,50 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="29.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:10" s="36" customFormat="1" ht="29.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="46" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>